<commit_message>
Se corrige rango de edad
</commit_message>
<xml_diff>
--- a/data_preprocesada_N1/edad_madrid_2021.xlsx
+++ b/data_preprocesada_N1/edad_madrid_2021.xlsx
@@ -31,7 +31,7 @@
     <t>0-14</t>
   </si>
   <si>
-    <t>15-19</t>
+    <t>15-29</t>
   </si>
   <si>
     <t>30-44</t>
@@ -833,7 +833,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>622</v>
+        <v>3834</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -847,7 +847,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>9564</v>
+        <v>6352</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -917,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>1127</v>
+        <v>8188</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -931,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>22475</v>
+        <v>15414</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1001,7 +1001,7 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>268</v>
+        <v>2030</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1015,7 +1015,7 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <v>4900</v>
+        <v>3138</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1085,7 +1085,7 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>481</v>
+        <v>3268</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -1099,7 +1099,7 @@
         <v>6</v>
       </c>
       <c r="B22">
-        <v>8115</v>
+        <v>5328</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
@@ -1169,7 +1169,7 @@
         <v>5</v>
       </c>
       <c r="B27">
-        <v>775</v>
+        <v>5927</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -1183,7 +1183,7 @@
         <v>6</v>
       </c>
       <c r="B28">
-        <v>15620</v>
+        <v>10468</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
@@ -1253,7 +1253,7 @@
         <v>5</v>
       </c>
       <c r="B33">
-        <v>211</v>
+        <v>1812</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
@@ -1267,7 +1267,7 @@
         <v>6</v>
       </c>
       <c r="B34">
-        <v>3913</v>
+        <v>2312</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
@@ -1337,7 +1337,7 @@
         <v>5</v>
       </c>
       <c r="B39">
-        <v>890</v>
+        <v>3216</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
@@ -1351,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="B40">
-        <v>7130</v>
+        <v>4804</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
@@ -1421,7 +1421,7 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <v>1286</v>
+        <v>5325</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
@@ -1435,7 +1435,7 @@
         <v>6</v>
       </c>
       <c r="B46">
-        <v>11954</v>
+        <v>7915</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -1505,7 +1505,7 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>562</v>
+        <v>2693</v>
       </c>
       <c r="C51" t="s">
         <v>18</v>
@@ -1519,7 +1519,7 @@
         <v>6</v>
       </c>
       <c r="B52">
-        <v>7291</v>
+        <v>5160</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -1589,7 +1589,7 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>1035</v>
+        <v>3066</v>
       </c>
       <c r="C57" t="s">
         <v>19</v>
@@ -1603,7 +1603,7 @@
         <v>6</v>
       </c>
       <c r="B58">
-        <v>6686</v>
+        <v>4655</v>
       </c>
       <c r="C58" t="s">
         <v>19</v>
@@ -1673,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="B63">
-        <v>1212</v>
+        <v>4315</v>
       </c>
       <c r="C63" t="s">
         <v>20</v>
@@ -1687,7 +1687,7 @@
         <v>6</v>
       </c>
       <c r="B64">
-        <v>10056</v>
+        <v>6953</v>
       </c>
       <c r="C64" t="s">
         <v>20</v>
@@ -1757,7 +1757,7 @@
         <v>5</v>
       </c>
       <c r="B69">
-        <v>679</v>
+        <v>3782</v>
       </c>
       <c r="C69" t="s">
         <v>21</v>
@@ -1771,7 +1771,7 @@
         <v>6</v>
       </c>
       <c r="B70">
-        <v>9671</v>
+        <v>6568</v>
       </c>
       <c r="C70" t="s">
         <v>21</v>
@@ -1841,7 +1841,7 @@
         <v>5</v>
       </c>
       <c r="B75">
-        <v>101</v>
+        <v>286</v>
       </c>
       <c r="C75" t="s">
         <v>22</v>
@@ -1855,7 +1855,7 @@
         <v>6</v>
       </c>
       <c r="B76">
-        <v>554</v>
+        <v>369</v>
       </c>
       <c r="C76" t="s">
         <v>22</v>
@@ -1925,7 +1925,7 @@
         <v>5</v>
       </c>
       <c r="B81">
-        <v>1109</v>
+        <v>4811</v>
       </c>
       <c r="C81" t="s">
         <v>23</v>
@@ -1939,7 +1939,7 @@
         <v>6</v>
       </c>
       <c r="B82">
-        <v>10570</v>
+        <v>6868</v>
       </c>
       <c r="C82" t="s">
         <v>23</v>
@@ -2009,7 +2009,7 @@
         <v>5</v>
       </c>
       <c r="B87">
-        <v>790</v>
+        <v>2684</v>
       </c>
       <c r="C87" t="s">
         <v>24</v>
@@ -2023,7 +2023,7 @@
         <v>6</v>
       </c>
       <c r="B88">
-        <v>6092</v>
+        <v>4198</v>
       </c>
       <c r="C88" t="s">
         <v>24</v>
@@ -2093,7 +2093,7 @@
         <v>5</v>
       </c>
       <c r="B93">
-        <v>963</v>
+        <v>2982</v>
       </c>
       <c r="C93" t="s">
         <v>25</v>
@@ -2107,7 +2107,7 @@
         <v>6</v>
       </c>
       <c r="B94">
-        <v>6011</v>
+        <v>3992</v>
       </c>
       <c r="C94" t="s">
         <v>25</v>
@@ -2177,7 +2177,7 @@
         <v>5</v>
       </c>
       <c r="B99">
-        <v>799</v>
+        <v>3111</v>
       </c>
       <c r="C99" t="s">
         <v>26</v>
@@ -2191,7 +2191,7 @@
         <v>6</v>
       </c>
       <c r="B100">
-        <v>6823</v>
+        <v>4511</v>
       </c>
       <c r="C100" t="s">
         <v>26</v>
@@ -2261,7 +2261,7 @@
         <v>5</v>
       </c>
       <c r="B105">
-        <v>229</v>
+        <v>1009</v>
       </c>
       <c r="C105" t="s">
         <v>27</v>
@@ -2275,7 +2275,7 @@
         <v>6</v>
       </c>
       <c r="B106">
-        <v>2123</v>
+        <v>1343</v>
       </c>
       <c r="C106" t="s">
         <v>27</v>
@@ -2345,7 +2345,7 @@
         <v>5</v>
       </c>
       <c r="B111">
-        <v>691</v>
+        <v>2249</v>
       </c>
       <c r="C111" t="s">
         <v>28</v>
@@ -2359,7 +2359,7 @@
         <v>6</v>
       </c>
       <c r="B112">
-        <v>4122</v>
+        <v>2564</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -2429,7 +2429,7 @@
         <v>5</v>
       </c>
       <c r="B117">
-        <v>613</v>
+        <v>2736</v>
       </c>
       <c r="C117" t="s">
         <v>29</v>
@@ -2443,7 +2443,7 @@
         <v>6</v>
       </c>
       <c r="B118">
-        <v>5237</v>
+        <v>3114</v>
       </c>
       <c r="C118" t="s">
         <v>29</v>
@@ -2513,7 +2513,7 @@
         <v>5</v>
       </c>
       <c r="B123">
-        <v>1043</v>
+        <v>5180</v>
       </c>
       <c r="C123" t="s">
         <v>30</v>
@@ -2527,7 +2527,7 @@
         <v>6</v>
       </c>
       <c r="B124">
-        <v>10587</v>
+        <v>6450</v>
       </c>
       <c r="C124" t="s">
         <v>30</v>
@@ -2597,7 +2597,7 @@
         <v>5</v>
       </c>
       <c r="B129">
-        <v>727</v>
+        <v>3077</v>
       </c>
       <c r="C129" t="s">
         <v>31</v>
@@ -2611,7 +2611,7 @@
         <v>6</v>
       </c>
       <c r="B130">
-        <v>7129</v>
+        <v>4779</v>
       </c>
       <c r="C130" t="s">
         <v>31</v>
@@ -2681,7 +2681,7 @@
         <v>5</v>
       </c>
       <c r="B135">
-        <v>1594</v>
+        <v>6711</v>
       </c>
       <c r="C135" t="s">
         <v>32</v>
@@ -2695,7 +2695,7 @@
         <v>6</v>
       </c>
       <c r="B136">
-        <v>14387</v>
+        <v>9270</v>
       </c>
       <c r="C136" t="s">
         <v>32</v>
@@ -2765,7 +2765,7 @@
         <v>5</v>
       </c>
       <c r="B141">
-        <v>803</v>
+        <v>3937</v>
       </c>
       <c r="C141" t="s">
         <v>33</v>
@@ -2779,7 +2779,7 @@
         <v>6</v>
       </c>
       <c r="B142">
-        <v>7635</v>
+        <v>4501</v>
       </c>
       <c r="C142" t="s">
         <v>33</v>
@@ -2849,7 +2849,7 @@
         <v>5</v>
       </c>
       <c r="B147">
-        <v>826</v>
+        <v>3677</v>
       </c>
       <c r="C147" t="s">
         <v>34</v>
@@ -2863,7 +2863,7 @@
         <v>6</v>
       </c>
       <c r="B148">
-        <v>6165</v>
+        <v>3314</v>
       </c>
       <c r="C148" t="s">
         <v>34</v>
@@ -2933,7 +2933,7 @@
         <v>5</v>
       </c>
       <c r="B153">
-        <v>780</v>
+        <v>2992</v>
       </c>
       <c r="C153" t="s">
         <v>35</v>
@@ -2947,7 +2947,7 @@
         <v>6</v>
       </c>
       <c r="B154">
-        <v>5610</v>
+        <v>3398</v>
       </c>
       <c r="C154" t="s">
         <v>35</v>
@@ -3017,7 +3017,7 @@
         <v>5</v>
       </c>
       <c r="B159">
-        <v>1157</v>
+        <v>5119</v>
       </c>
       <c r="C159" t="s">
         <v>36</v>
@@ -3031,7 +3031,7 @@
         <v>6</v>
       </c>
       <c r="B160">
-        <v>12231</v>
+        <v>8269</v>
       </c>
       <c r="C160" t="s">
         <v>36</v>
@@ -3101,7 +3101,7 @@
         <v>5</v>
       </c>
       <c r="B165">
-        <v>659</v>
+        <v>2608</v>
       </c>
       <c r="C165" t="s">
         <v>37</v>
@@ -3115,7 +3115,7 @@
         <v>6</v>
       </c>
       <c r="B166">
-        <v>6288</v>
+        <v>4339</v>
       </c>
       <c r="C166" t="s">
         <v>37</v>
@@ -3185,7 +3185,7 @@
         <v>5</v>
       </c>
       <c r="B171">
-        <v>1431</v>
+        <v>4586</v>
       </c>
       <c r="C171" t="s">
         <v>38</v>
@@ -3199,7 +3199,7 @@
         <v>6</v>
       </c>
       <c r="B172">
-        <v>9257</v>
+        <v>6102</v>
       </c>
       <c r="C172" t="s">
         <v>38</v>
@@ -3269,7 +3269,7 @@
         <v>5</v>
       </c>
       <c r="B177">
-        <v>1182</v>
+        <v>3807</v>
       </c>
       <c r="C177" t="s">
         <v>39</v>
@@ -3283,7 +3283,7 @@
         <v>6</v>
       </c>
       <c r="B178">
-        <v>7545</v>
+        <v>4920</v>
       </c>
       <c r="C178" t="s">
         <v>39</v>
@@ -3353,7 +3353,7 @@
         <v>5</v>
       </c>
       <c r="B183">
-        <v>710</v>
+        <v>2826</v>
       </c>
       <c r="C183" t="s">
         <v>40</v>
@@ -3367,7 +3367,7 @@
         <v>6</v>
       </c>
       <c r="B184">
-        <v>5793</v>
+        <v>3677</v>
       </c>
       <c r="C184" t="s">
         <v>40</v>
@@ -3437,7 +3437,7 @@
         <v>5</v>
       </c>
       <c r="B189">
-        <v>1054</v>
+        <v>5037</v>
       </c>
       <c r="C189" t="s">
         <v>41</v>
@@ -3451,7 +3451,7 @@
         <v>6</v>
       </c>
       <c r="B190">
-        <v>11586</v>
+        <v>7603</v>
       </c>
       <c r="C190" t="s">
         <v>41</v>
@@ -3521,7 +3521,7 @@
         <v>5</v>
       </c>
       <c r="B195">
-        <v>1168</v>
+        <v>5619</v>
       </c>
       <c r="C195" t="s">
         <v>42</v>
@@ -3535,7 +3535,7 @@
         <v>6</v>
       </c>
       <c r="B196">
-        <v>13040</v>
+        <v>8589</v>
       </c>
       <c r="C196" t="s">
         <v>42</v>
@@ -3605,7 +3605,7 @@
         <v>5</v>
       </c>
       <c r="B201">
-        <v>597</v>
+        <v>2999</v>
       </c>
       <c r="C201" t="s">
         <v>43</v>
@@ -3619,7 +3619,7 @@
         <v>6</v>
       </c>
       <c r="B202">
-        <v>7641</v>
+        <v>5239</v>
       </c>
       <c r="C202" t="s">
         <v>43</v>
@@ -3689,7 +3689,7 @@
         <v>5</v>
       </c>
       <c r="B207">
-        <v>1008</v>
+        <v>3978</v>
       </c>
       <c r="C207" t="s">
         <v>44</v>
@@ -3703,7 +3703,7 @@
         <v>6</v>
       </c>
       <c r="B208">
-        <v>8474</v>
+        <v>5504</v>
       </c>
       <c r="C208" t="s">
         <v>44</v>
@@ -3773,7 +3773,7 @@
         <v>5</v>
       </c>
       <c r="B213">
-        <v>997</v>
+        <v>4546</v>
       </c>
       <c r="C213" t="s">
         <v>45</v>
@@ -3787,7 +3787,7 @@
         <v>6</v>
       </c>
       <c r="B214">
-        <v>10702</v>
+        <v>7153</v>
       </c>
       <c r="C214" t="s">
         <v>45</v>
@@ -3857,7 +3857,7 @@
         <v>5</v>
       </c>
       <c r="B219">
-        <v>927</v>
+        <v>4301</v>
       </c>
       <c r="C219" t="s">
         <v>46</v>
@@ -3871,7 +3871,7 @@
         <v>6</v>
       </c>
       <c r="B220">
-        <v>10035</v>
+        <v>6661</v>
       </c>
       <c r="C220" t="s">
         <v>46</v>
@@ -3941,7 +3941,7 @@
         <v>5</v>
       </c>
       <c r="B225">
-        <v>722</v>
+        <v>4081</v>
       </c>
       <c r="C225" t="s">
         <v>47</v>
@@ -3955,7 +3955,7 @@
         <v>6</v>
       </c>
       <c r="B226">
-        <v>8293</v>
+        <v>4934</v>
       </c>
       <c r="C226" t="s">
         <v>47</v>
@@ -4025,7 +4025,7 @@
         <v>5</v>
       </c>
       <c r="B231">
-        <v>823</v>
+        <v>4210</v>
       </c>
       <c r="C231" t="s">
         <v>48</v>
@@ -4039,7 +4039,7 @@
         <v>6</v>
       </c>
       <c r="B232">
-        <v>9028</v>
+        <v>5641</v>
       </c>
       <c r="C232" t="s">
         <v>48</v>
@@ -4109,7 +4109,7 @@
         <v>5</v>
       </c>
       <c r="B237">
-        <v>802</v>
+        <v>4071</v>
       </c>
       <c r="C237" t="s">
         <v>49</v>
@@ -4123,7 +4123,7 @@
         <v>6</v>
       </c>
       <c r="B238">
-        <v>9724</v>
+        <v>6455</v>
       </c>
       <c r="C238" t="s">
         <v>49</v>
@@ -4193,7 +4193,7 @@
         <v>5</v>
       </c>
       <c r="B243">
-        <v>738</v>
+        <v>3206</v>
       </c>
       <c r="C243" t="s">
         <v>50</v>
@@ -4207,7 +4207,7 @@
         <v>6</v>
       </c>
       <c r="B244">
-        <v>6583</v>
+        <v>4115</v>
       </c>
       <c r="C244" t="s">
         <v>50</v>
@@ -4277,7 +4277,7 @@
         <v>5</v>
       </c>
       <c r="B249">
-        <v>934</v>
+        <v>4322</v>
       </c>
       <c r="C249" t="s">
         <v>51</v>
@@ -4291,7 +4291,7 @@
         <v>6</v>
       </c>
       <c r="B250">
-        <v>9800</v>
+        <v>6412</v>
       </c>
       <c r="C250" t="s">
         <v>51</v>
@@ -4361,7 +4361,7 @@
         <v>5</v>
       </c>
       <c r="B255">
-        <v>820</v>
+        <v>3281</v>
       </c>
       <c r="C255" t="s">
         <v>52</v>
@@ -4375,7 +4375,7 @@
         <v>6</v>
       </c>
       <c r="B256">
-        <v>6269</v>
+        <v>3808</v>
       </c>
       <c r="C256" t="s">
         <v>52</v>
@@ -4445,7 +4445,7 @@
         <v>5</v>
       </c>
       <c r="B261">
-        <v>128</v>
+        <v>466</v>
       </c>
       <c r="C261" t="s">
         <v>53</v>
@@ -4459,7 +4459,7 @@
         <v>6</v>
       </c>
       <c r="B262">
-        <v>1027</v>
+        <v>689</v>
       </c>
       <c r="C262" t="s">
         <v>53</v>
@@ -4529,7 +4529,7 @@
         <v>5</v>
       </c>
       <c r="B267">
-        <v>179</v>
+        <v>537</v>
       </c>
       <c r="C267" t="s">
         <v>54</v>
@@ -4543,7 +4543,7 @@
         <v>6</v>
       </c>
       <c r="B268">
-        <v>853</v>
+        <v>495</v>
       </c>
       <c r="C268" t="s">
         <v>54</v>
@@ -4613,7 +4613,7 @@
         <v>5</v>
       </c>
       <c r="B273">
-        <v>1906</v>
+        <v>6099</v>
       </c>
       <c r="C273" t="s">
         <v>55</v>
@@ -4627,7 +4627,7 @@
         <v>6</v>
       </c>
       <c r="B274">
-        <v>12576</v>
+        <v>8383</v>
       </c>
       <c r="C274" t="s">
         <v>55</v>
@@ -4697,7 +4697,7 @@
         <v>5</v>
       </c>
       <c r="B279">
-        <v>1476</v>
+        <v>5890</v>
       </c>
       <c r="C279" t="s">
         <v>56</v>
@@ -4711,7 +4711,7 @@
         <v>6</v>
       </c>
       <c r="B280">
-        <v>14301</v>
+        <v>9887</v>
       </c>
       <c r="C280" t="s">
         <v>56</v>
@@ -4781,7 +4781,7 @@
         <v>5</v>
       </c>
       <c r="B285">
-        <v>1029</v>
+        <v>3769</v>
       </c>
       <c r="C285" t="s">
         <v>57</v>
@@ -4795,7 +4795,7 @@
         <v>6</v>
       </c>
       <c r="B286">
-        <v>8723</v>
+        <v>5983</v>
       </c>
       <c r="C286" t="s">
         <v>57</v>
@@ -4865,7 +4865,7 @@
         <v>5</v>
       </c>
       <c r="B291">
-        <v>3518</v>
+        <v>9337</v>
       </c>
       <c r="C291" t="s">
         <v>58</v>
@@ -4879,7 +4879,7 @@
         <v>6</v>
       </c>
       <c r="B292">
-        <v>20422</v>
+        <v>14603</v>
       </c>
       <c r="C292" t="s">
         <v>58</v>
@@ -4949,7 +4949,7 @@
         <v>5</v>
       </c>
       <c r="B297">
-        <v>2272</v>
+        <v>6255</v>
       </c>
       <c r="C297" t="s">
         <v>59</v>
@@ -4963,7 +4963,7 @@
         <v>6</v>
       </c>
       <c r="B298">
-        <v>10201</v>
+        <v>6218</v>
       </c>
       <c r="C298" t="s">
         <v>59</v>
@@ -5033,7 +5033,7 @@
         <v>5</v>
       </c>
       <c r="B303">
-        <v>1297</v>
+        <v>2484</v>
       </c>
       <c r="C303" t="s">
         <v>60</v>
@@ -5047,7 +5047,7 @@
         <v>6</v>
       </c>
       <c r="B304">
-        <v>5474</v>
+        <v>4287</v>
       </c>
       <c r="C304" t="s">
         <v>60</v>
@@ -5117,7 +5117,7 @@
         <v>5</v>
       </c>
       <c r="B309">
-        <v>525</v>
+        <v>1907</v>
       </c>
       <c r="C309" t="s">
         <v>61</v>
@@ -5131,7 +5131,7 @@
         <v>6</v>
       </c>
       <c r="B310">
-        <v>3894</v>
+        <v>2512</v>
       </c>
       <c r="C310" t="s">
         <v>61</v>
@@ -5201,7 +5201,7 @@
         <v>5</v>
       </c>
       <c r="B315">
-        <v>839</v>
+        <v>4188</v>
       </c>
       <c r="C315" t="s">
         <v>62</v>
@@ -5215,7 +5215,7 @@
         <v>6</v>
       </c>
       <c r="B316">
-        <v>8565</v>
+        <v>5216</v>
       </c>
       <c r="C316" t="s">
         <v>62</v>
@@ -5285,7 +5285,7 @@
         <v>5</v>
       </c>
       <c r="B321">
-        <v>833</v>
+        <v>2916</v>
       </c>
       <c r="C321" t="s">
         <v>63</v>
@@ -5299,7 +5299,7 @@
         <v>6</v>
       </c>
       <c r="B322">
-        <v>5078</v>
+        <v>2995</v>
       </c>
       <c r="C322" t="s">
         <v>63</v>
@@ -5369,7 +5369,7 @@
         <v>5</v>
       </c>
       <c r="B327">
-        <v>1196</v>
+        <v>4378</v>
       </c>
       <c r="C327" t="s">
         <v>64</v>
@@ -5383,7 +5383,7 @@
         <v>6</v>
       </c>
       <c r="B328">
-        <v>9421</v>
+        <v>6239</v>
       </c>
       <c r="C328" t="s">
         <v>64</v>
@@ -5453,7 +5453,7 @@
         <v>5</v>
       </c>
       <c r="B333">
-        <v>610</v>
+        <v>1319</v>
       </c>
       <c r="C333" t="s">
         <v>65</v>
@@ -5467,7 +5467,7 @@
         <v>6</v>
       </c>
       <c r="B334">
-        <v>1899</v>
+        <v>1190</v>
       </c>
       <c r="C334" t="s">
         <v>65</v>
@@ -5537,7 +5537,7 @@
         <v>5</v>
       </c>
       <c r="B339">
-        <v>217</v>
+        <v>530</v>
       </c>
       <c r="C339" t="s">
         <v>66</v>
@@ -5551,7 +5551,7 @@
         <v>6</v>
       </c>
       <c r="B340">
-        <v>815</v>
+        <v>502</v>
       </c>
       <c r="C340" t="s">
         <v>66</v>
@@ -5621,7 +5621,7 @@
         <v>5</v>
       </c>
       <c r="B345">
-        <v>2072</v>
+        <v>5601</v>
       </c>
       <c r="C345" t="s">
         <v>67</v>
@@ -5635,7 +5635,7 @@
         <v>6</v>
       </c>
       <c r="B346">
-        <v>7968</v>
+        <v>4439</v>
       </c>
       <c r="C346" t="s">
         <v>67</v>
@@ -5705,7 +5705,7 @@
         <v>5</v>
       </c>
       <c r="B351">
-        <v>927</v>
+        <v>3354</v>
       </c>
       <c r="C351" t="s">
         <v>68</v>
@@ -5719,7 +5719,7 @@
         <v>6</v>
       </c>
       <c r="B352">
-        <v>5880</v>
+        <v>3453</v>
       </c>
       <c r="C352" t="s">
         <v>68</v>
@@ -5789,7 +5789,7 @@
         <v>5</v>
       </c>
       <c r="B357">
-        <v>1602</v>
+        <v>6945</v>
       </c>
       <c r="C357" t="s">
         <v>69</v>
@@ -5803,7 +5803,7 @@
         <v>6</v>
       </c>
       <c r="B358">
-        <v>15135</v>
+        <v>9792</v>
       </c>
       <c r="C358" t="s">
         <v>69</v>
@@ -5873,7 +5873,7 @@
         <v>5</v>
       </c>
       <c r="B363">
-        <v>1643</v>
+        <v>6227</v>
       </c>
       <c r="C363" t="s">
         <v>70</v>
@@ -5887,7 +5887,7 @@
         <v>6</v>
       </c>
       <c r="B364">
-        <v>11795</v>
+        <v>7211</v>
       </c>
       <c r="C364" t="s">
         <v>70</v>
@@ -5957,7 +5957,7 @@
         <v>5</v>
       </c>
       <c r="B369">
-        <v>2481</v>
+        <v>9147</v>
       </c>
       <c r="C369" t="s">
         <v>71</v>
@@ -5971,7 +5971,7 @@
         <v>6</v>
       </c>
       <c r="B370">
-        <v>19567</v>
+        <v>12901</v>
       </c>
       <c r="C370" t="s">
         <v>71</v>
@@ -6041,7 +6041,7 @@
         <v>5</v>
       </c>
       <c r="B375">
-        <v>797</v>
+        <v>3033</v>
       </c>
       <c r="C375" t="s">
         <v>72</v>
@@ -6055,7 +6055,7 @@
         <v>6</v>
       </c>
       <c r="B376">
-        <v>6368</v>
+        <v>4132</v>
       </c>
       <c r="C376" t="s">
         <v>72</v>
@@ -6125,7 +6125,7 @@
         <v>5</v>
       </c>
       <c r="B381">
-        <v>320</v>
+        <v>900</v>
       </c>
       <c r="C381" t="s">
         <v>73</v>
@@ -6139,7 +6139,7 @@
         <v>6</v>
       </c>
       <c r="B382">
-        <v>2008</v>
+        <v>1428</v>
       </c>
       <c r="C382" t="s">
         <v>73</v>
@@ -6209,7 +6209,7 @@
         <v>5</v>
       </c>
       <c r="B387">
-        <v>2198</v>
+        <v>7244</v>
       </c>
       <c r="C387" t="s">
         <v>74</v>
@@ -6223,7 +6223,7 @@
         <v>6</v>
       </c>
       <c r="B388">
-        <v>14197</v>
+        <v>9151</v>
       </c>
       <c r="C388" t="s">
         <v>74</v>
@@ -6293,7 +6293,7 @@
         <v>5</v>
       </c>
       <c r="B393">
-        <v>732</v>
+        <v>3292</v>
       </c>
       <c r="C393" t="s">
         <v>75</v>
@@ -6307,7 +6307,7 @@
         <v>6</v>
       </c>
       <c r="B394">
-        <v>7785</v>
+        <v>5225</v>
       </c>
       <c r="C394" t="s">
         <v>75</v>
@@ -6377,7 +6377,7 @@
         <v>5</v>
       </c>
       <c r="B399">
-        <v>1378</v>
+        <v>5630</v>
       </c>
       <c r="C399" t="s">
         <v>76</v>
@@ -6391,7 +6391,7 @@
         <v>6</v>
       </c>
       <c r="B400">
-        <v>12060</v>
+        <v>7808</v>
       </c>
       <c r="C400" t="s">
         <v>76</v>
@@ -6461,7 +6461,7 @@
         <v>5</v>
       </c>
       <c r="B405">
-        <v>1701</v>
+        <v>6695</v>
       </c>
       <c r="C405" t="s">
         <v>77</v>
@@ -6475,7 +6475,7 @@
         <v>6</v>
       </c>
       <c r="B406">
-        <v>13889</v>
+        <v>8895</v>
       </c>
       <c r="C406" t="s">
         <v>77</v>
@@ -6545,7 +6545,7 @@
         <v>5</v>
       </c>
       <c r="B411">
-        <v>2024</v>
+        <v>7753</v>
       </c>
       <c r="C411" t="s">
         <v>78</v>
@@ -6559,7 +6559,7 @@
         <v>6</v>
       </c>
       <c r="B412">
-        <v>15796</v>
+        <v>10067</v>
       </c>
       <c r="C412" t="s">
         <v>78</v>
@@ -6629,7 +6629,7 @@
         <v>5</v>
       </c>
       <c r="B417">
-        <v>1868</v>
+        <v>6596</v>
       </c>
       <c r="C417" t="s">
         <v>79</v>
@@ -6643,7 +6643,7 @@
         <v>6</v>
       </c>
       <c r="B418">
-        <v>12423</v>
+        <v>7695</v>
       </c>
       <c r="C418" t="s">
         <v>79</v>
@@ -6713,7 +6713,7 @@
         <v>5</v>
       </c>
       <c r="B423">
-        <v>2894</v>
+        <v>7788</v>
       </c>
       <c r="C423" t="s">
         <v>80</v>
@@ -6727,7 +6727,7 @@
         <v>6</v>
       </c>
       <c r="B424">
-        <v>14456</v>
+        <v>9562</v>
       </c>
       <c r="C424" t="s">
         <v>80</v>
@@ -6797,7 +6797,7 @@
         <v>5</v>
       </c>
       <c r="B429">
-        <v>1718</v>
+        <v>5488</v>
       </c>
       <c r="C429" t="s">
         <v>81</v>
@@ -6811,7 +6811,7 @@
         <v>6</v>
       </c>
       <c r="B430">
-        <v>10009</v>
+        <v>6239</v>
       </c>
       <c r="C430" t="s">
         <v>81</v>
@@ -6881,7 +6881,7 @@
         <v>5</v>
       </c>
       <c r="B435">
-        <v>1386</v>
+        <v>3729</v>
       </c>
       <c r="C435" t="s">
         <v>82</v>
@@ -6895,7 +6895,7 @@
         <v>6</v>
       </c>
       <c r="B436">
-        <v>6459</v>
+        <v>4116</v>
       </c>
       <c r="C436" t="s">
         <v>82</v>
@@ -6965,7 +6965,7 @@
         <v>5</v>
       </c>
       <c r="B441">
-        <v>807</v>
+        <v>2740</v>
       </c>
       <c r="C441" t="s">
         <v>83</v>
@@ -6979,7 +6979,7 @@
         <v>6</v>
       </c>
       <c r="B442">
-        <v>4986</v>
+        <v>3053</v>
       </c>
       <c r="C442" t="s">
         <v>83</v>
@@ -7049,7 +7049,7 @@
         <v>5</v>
       </c>
       <c r="B447">
-        <v>1590</v>
+        <v>4514</v>
       </c>
       <c r="C447" t="s">
         <v>84</v>
@@ -7063,7 +7063,7 @@
         <v>6</v>
       </c>
       <c r="B448">
-        <v>7541</v>
+        <v>4617</v>
       </c>
       <c r="C448" t="s">
         <v>84</v>
@@ -7133,7 +7133,7 @@
         <v>5</v>
       </c>
       <c r="B453">
-        <v>1115</v>
+        <v>3949</v>
       </c>
       <c r="C453" t="s">
         <v>85</v>
@@ -7147,7 +7147,7 @@
         <v>6</v>
       </c>
       <c r="B454">
-        <v>8129</v>
+        <v>5295</v>
       </c>
       <c r="C454" t="s">
         <v>85</v>
@@ -7217,7 +7217,7 @@
         <v>5</v>
       </c>
       <c r="B459">
-        <v>1092</v>
+        <v>4436</v>
       </c>
       <c r="C459" t="s">
         <v>86</v>
@@ -7231,7 +7231,7 @@
         <v>6</v>
       </c>
       <c r="B460">
-        <v>9492</v>
+        <v>6148</v>
       </c>
       <c r="C460" t="s">
         <v>86</v>
@@ -7301,7 +7301,7 @@
         <v>5</v>
       </c>
       <c r="B465">
-        <v>695</v>
+        <v>2658</v>
       </c>
       <c r="C465" t="s">
         <v>87</v>
@@ -7315,7 +7315,7 @@
         <v>6</v>
       </c>
       <c r="B466">
-        <v>4945</v>
+        <v>2982</v>
       </c>
       <c r="C466" t="s">
         <v>87</v>
@@ -7385,7 +7385,7 @@
         <v>5</v>
       </c>
       <c r="B471">
-        <v>799</v>
+        <v>3152</v>
       </c>
       <c r="C471" t="s">
         <v>88</v>
@@ -7399,7 +7399,7 @@
         <v>6</v>
       </c>
       <c r="B472">
-        <v>6571</v>
+        <v>4218</v>
       </c>
       <c r="C472" t="s">
         <v>88</v>
@@ -7469,7 +7469,7 @@
         <v>5</v>
       </c>
       <c r="B477">
-        <v>1769</v>
+        <v>6181</v>
       </c>
       <c r="C477" t="s">
         <v>89</v>
@@ -7483,7 +7483,7 @@
         <v>6</v>
       </c>
       <c r="B478">
-        <v>11627</v>
+        <v>7215</v>
       </c>
       <c r="C478" t="s">
         <v>89</v>
@@ -7553,7 +7553,7 @@
         <v>5</v>
       </c>
       <c r="B483">
-        <v>1973</v>
+        <v>8167</v>
       </c>
       <c r="C483" t="s">
         <v>90</v>
@@ -7567,7 +7567,7 @@
         <v>6</v>
       </c>
       <c r="B484">
-        <v>17058</v>
+        <v>10864</v>
       </c>
       <c r="C484" t="s">
         <v>90</v>
@@ -7637,7 +7637,7 @@
         <v>5</v>
       </c>
       <c r="B489">
-        <v>2096</v>
+        <v>7657</v>
       </c>
       <c r="C489" t="s">
         <v>91</v>
@@ -7651,7 +7651,7 @@
         <v>6</v>
       </c>
       <c r="B490">
-        <v>13003</v>
+        <v>7442</v>
       </c>
       <c r="C490" t="s">
         <v>91</v>
@@ -7721,7 +7721,7 @@
         <v>5</v>
       </c>
       <c r="B495">
-        <v>1999</v>
+        <v>7170</v>
       </c>
       <c r="C495" t="s">
         <v>92</v>
@@ -7735,7 +7735,7 @@
         <v>6</v>
       </c>
       <c r="B496">
-        <v>14042</v>
+        <v>8871</v>
       </c>
       <c r="C496" t="s">
         <v>92</v>
@@ -7805,7 +7805,7 @@
         <v>5</v>
       </c>
       <c r="B501">
-        <v>1284</v>
+        <v>4451</v>
       </c>
       <c r="C501" t="s">
         <v>93</v>
@@ -7819,7 +7819,7 @@
         <v>6</v>
       </c>
       <c r="B502">
-        <v>9365</v>
+        <v>6198</v>
       </c>
       <c r="C502" t="s">
         <v>93</v>
@@ -7889,7 +7889,7 @@
         <v>5</v>
       </c>
       <c r="B507">
-        <v>2058</v>
+        <v>8239</v>
       </c>
       <c r="C507" t="s">
         <v>94</v>
@@ -7903,7 +7903,7 @@
         <v>6</v>
       </c>
       <c r="B508">
-        <v>17089</v>
+        <v>10908</v>
       </c>
       <c r="C508" t="s">
         <v>94</v>
@@ -7973,7 +7973,7 @@
         <v>5</v>
       </c>
       <c r="B513">
-        <v>455</v>
+        <v>1393</v>
       </c>
       <c r="C513" t="s">
         <v>95</v>
@@ -7987,7 +7987,7 @@
         <v>6</v>
       </c>
       <c r="B514">
-        <v>2440</v>
+        <v>1502</v>
       </c>
       <c r="C514" t="s">
         <v>95</v>
@@ -8057,7 +8057,7 @@
         <v>5</v>
       </c>
       <c r="B519">
-        <v>570</v>
+        <v>1542</v>
       </c>
       <c r="C519" t="s">
         <v>96</v>
@@ -8071,7 +8071,7 @@
         <v>6</v>
       </c>
       <c r="B520">
-        <v>1774</v>
+        <v>802</v>
       </c>
       <c r="C520" t="s">
         <v>96</v>
@@ -8141,7 +8141,7 @@
         <v>5</v>
       </c>
       <c r="B525">
-        <v>1122</v>
+        <v>4241</v>
       </c>
       <c r="C525" t="s">
         <v>97</v>
@@ -8155,7 +8155,7 @@
         <v>6</v>
       </c>
       <c r="B526">
-        <v>7087</v>
+        <v>3968</v>
       </c>
       <c r="C526" t="s">
         <v>97</v>
@@ -8225,7 +8225,7 @@
         <v>5</v>
       </c>
       <c r="B531">
-        <v>677</v>
+        <v>2643</v>
       </c>
       <c r="C531" t="s">
         <v>98</v>
@@ -8239,7 +8239,7 @@
         <v>6</v>
       </c>
       <c r="B532">
-        <v>5044</v>
+        <v>3078</v>
       </c>
       <c r="C532" t="s">
         <v>98</v>
@@ -8309,7 +8309,7 @@
         <v>5</v>
       </c>
       <c r="B537">
-        <v>714</v>
+        <v>2627</v>
       </c>
       <c r="C537" t="s">
         <v>99</v>
@@ -8323,7 +8323,7 @@
         <v>6</v>
       </c>
       <c r="B538">
-        <v>5370</v>
+        <v>3457</v>
       </c>
       <c r="C538" t="s">
         <v>99</v>
@@ -8393,7 +8393,7 @@
         <v>5</v>
       </c>
       <c r="B543">
-        <v>579</v>
+        <v>2144</v>
       </c>
       <c r="C543" t="s">
         <v>100</v>
@@ -8407,7 +8407,7 @@
         <v>6</v>
       </c>
       <c r="B544">
-        <v>4740</v>
+        <v>3175</v>
       </c>
       <c r="C544" t="s">
         <v>100</v>
@@ -8477,7 +8477,7 @@
         <v>5</v>
       </c>
       <c r="B549">
-        <v>1900</v>
+        <v>7559</v>
       </c>
       <c r="C549" t="s">
         <v>101</v>
@@ -8491,7 +8491,7 @@
         <v>6</v>
       </c>
       <c r="B550">
-        <v>16125</v>
+        <v>10466</v>
       </c>
       <c r="C550" t="s">
         <v>101</v>
@@ -8561,7 +8561,7 @@
         <v>5</v>
       </c>
       <c r="B555">
-        <v>2678</v>
+        <v>10077</v>
       </c>
       <c r="C555" t="s">
         <v>102</v>
@@ -8575,7 +8575,7 @@
         <v>6</v>
       </c>
       <c r="B556">
-        <v>20778</v>
+        <v>13379</v>
       </c>
       <c r="C556" t="s">
         <v>102</v>
@@ -8645,7 +8645,7 @@
         <v>5</v>
       </c>
       <c r="B561">
-        <v>854</v>
+        <v>3830</v>
       </c>
       <c r="C561" t="s">
         <v>103</v>
@@ -8659,7 +8659,7 @@
         <v>6</v>
       </c>
       <c r="B562">
-        <v>8608</v>
+        <v>5632</v>
       </c>
       <c r="C562" t="s">
         <v>103</v>
@@ -8729,7 +8729,7 @@
         <v>5</v>
       </c>
       <c r="B567">
-        <v>832</v>
+        <v>3001</v>
       </c>
       <c r="C567" t="s">
         <v>104</v>
@@ -8743,7 +8743,7 @@
         <v>6</v>
       </c>
       <c r="B568">
-        <v>6510</v>
+        <v>4341</v>
       </c>
       <c r="C568" t="s">
         <v>104</v>
@@ -8813,7 +8813,7 @@
         <v>5</v>
       </c>
       <c r="B573">
-        <v>715</v>
+        <v>2372</v>
       </c>
       <c r="C573" t="s">
         <v>105</v>
@@ -8827,7 +8827,7 @@
         <v>6</v>
       </c>
       <c r="B574">
-        <v>5018</v>
+        <v>3361</v>
       </c>
       <c r="C574" t="s">
         <v>105</v>
@@ -8897,7 +8897,7 @@
         <v>5</v>
       </c>
       <c r="B579">
-        <v>661</v>
+        <v>1961</v>
       </c>
       <c r="C579" t="s">
         <v>106</v>
@@ -8911,7 +8911,7 @@
         <v>6</v>
       </c>
       <c r="B580">
-        <v>3513</v>
+        <v>2213</v>
       </c>
       <c r="C580" t="s">
         <v>106</v>
@@ -8981,7 +8981,7 @@
         <v>5</v>
       </c>
       <c r="B585">
-        <v>313</v>
+        <v>900</v>
       </c>
       <c r="C585" t="s">
         <v>107</v>
@@ -8995,7 +8995,7 @@
         <v>6</v>
       </c>
       <c r="B586">
-        <v>1826</v>
+        <v>1239</v>
       </c>
       <c r="C586" t="s">
         <v>107</v>
@@ -9065,7 +9065,7 @@
         <v>5</v>
       </c>
       <c r="B591">
-        <v>94</v>
+        <v>253</v>
       </c>
       <c r="C591" t="s">
         <v>108</v>
@@ -9079,7 +9079,7 @@
         <v>6</v>
       </c>
       <c r="B592">
-        <v>440</v>
+        <v>281</v>
       </c>
       <c r="C592" t="s">
         <v>108</v>
@@ -9149,7 +9149,7 @@
         <v>5</v>
       </c>
       <c r="B597">
-        <v>1397</v>
+        <v>4013</v>
       </c>
       <c r="C597" t="s">
         <v>109</v>
@@ -9163,7 +9163,7 @@
         <v>6</v>
       </c>
       <c r="B598">
-        <v>5989</v>
+        <v>3373</v>
       </c>
       <c r="C598" t="s">
         <v>109</v>
@@ -9233,7 +9233,7 @@
         <v>5</v>
       </c>
       <c r="B603">
-        <v>579</v>
+        <v>1326</v>
       </c>
       <c r="C603" t="s">
         <v>110</v>
@@ -9247,7 +9247,7 @@
         <v>6</v>
       </c>
       <c r="B604">
-        <v>1795</v>
+        <v>1048</v>
       </c>
       <c r="C604" t="s">
         <v>110</v>
@@ -9317,7 +9317,7 @@
         <v>5</v>
       </c>
       <c r="B609">
-        <v>1062</v>
+        <v>2916</v>
       </c>
       <c r="C609" t="s">
         <v>111</v>
@@ -9331,7 +9331,7 @@
         <v>6</v>
       </c>
       <c r="B610">
-        <v>4174</v>
+        <v>2320</v>
       </c>
       <c r="C610" t="s">
         <v>111</v>
@@ -9401,7 +9401,7 @@
         <v>5</v>
       </c>
       <c r="B615">
-        <v>1639</v>
+        <v>5380</v>
       </c>
       <c r="C615" t="s">
         <v>112</v>
@@ -9415,7 +9415,7 @@
         <v>6</v>
       </c>
       <c r="B616">
-        <v>11302</v>
+        <v>7561</v>
       </c>
       <c r="C616" t="s">
         <v>112</v>
@@ -9485,7 +9485,7 @@
         <v>5</v>
       </c>
       <c r="B621">
-        <v>2191</v>
+        <v>7426</v>
       </c>
       <c r="C621" t="s">
         <v>113</v>
@@ -9499,7 +9499,7 @@
         <v>6</v>
       </c>
       <c r="B622">
-        <v>15436</v>
+        <v>10201</v>
       </c>
       <c r="C622" t="s">
         <v>113</v>
@@ -9569,7 +9569,7 @@
         <v>5</v>
       </c>
       <c r="B627">
-        <v>797</v>
+        <v>2644</v>
       </c>
       <c r="C627" t="s">
         <v>114</v>
@@ -9583,7 +9583,7 @@
         <v>6</v>
       </c>
       <c r="B628">
-        <v>4668</v>
+        <v>2821</v>
       </c>
       <c r="C628" t="s">
         <v>114</v>
@@ -9653,7 +9653,7 @@
         <v>5</v>
       </c>
       <c r="B633">
-        <v>3713</v>
+        <v>8727</v>
       </c>
       <c r="C633" t="s">
         <v>115</v>
@@ -9667,7 +9667,7 @@
         <v>6</v>
       </c>
       <c r="B634">
-        <v>21495</v>
+        <v>16481</v>
       </c>
       <c r="C634" t="s">
         <v>115</v>
@@ -9737,7 +9737,7 @@
         <v>5</v>
       </c>
       <c r="B639">
-        <v>2468</v>
+        <v>8257</v>
       </c>
       <c r="C639" t="s">
         <v>116</v>
@@ -9751,7 +9751,7 @@
         <v>6</v>
       </c>
       <c r="B640">
-        <v>15532</v>
+        <v>9743</v>
       </c>
       <c r="C640" t="s">
         <v>116</v>
@@ -9821,7 +9821,7 @@
         <v>5</v>
       </c>
       <c r="B645">
-        <v>934</v>
+        <v>3419</v>
       </c>
       <c r="C645" t="s">
         <v>117</v>
@@ -9835,7 +9835,7 @@
         <v>6</v>
       </c>
       <c r="B646">
-        <v>6411</v>
+        <v>3926</v>
       </c>
       <c r="C646" t="s">
         <v>117</v>
@@ -9905,7 +9905,7 @@
         <v>5</v>
       </c>
       <c r="B651">
-        <v>1387</v>
+        <v>3277</v>
       </c>
       <c r="C651" t="s">
         <v>118</v>
@@ -9919,7 +9919,7 @@
         <v>6</v>
       </c>
       <c r="B652">
-        <v>7031</v>
+        <v>5141</v>
       </c>
       <c r="C652" t="s">
         <v>118</v>
@@ -9989,7 +9989,7 @@
         <v>5</v>
       </c>
       <c r="B657">
-        <v>2144</v>
+        <v>7041</v>
       </c>
       <c r="C657" t="s">
         <v>119</v>
@@ -10003,7 +10003,7 @@
         <v>6</v>
       </c>
       <c r="B658">
-        <v>11899</v>
+        <v>7002</v>
       </c>
       <c r="C658" t="s">
         <v>119</v>
@@ -10073,7 +10073,7 @@
         <v>5</v>
       </c>
       <c r="B663">
-        <v>1354</v>
+        <v>5168</v>
       </c>
       <c r="C663" t="s">
         <v>120</v>
@@ -10087,7 +10087,7 @@
         <v>6</v>
       </c>
       <c r="B664">
-        <v>10594</v>
+        <v>6780</v>
       </c>
       <c r="C664" t="s">
         <v>120</v>
@@ -10157,7 +10157,7 @@
         <v>5</v>
       </c>
       <c r="B669">
-        <v>2223</v>
+        <v>7023</v>
       </c>
       <c r="C669" t="s">
         <v>121</v>
@@ -10171,7 +10171,7 @@
         <v>6</v>
       </c>
       <c r="B670">
-        <v>13273</v>
+        <v>8473</v>
       </c>
       <c r="C670" t="s">
         <v>121</v>
@@ -10241,7 +10241,7 @@
         <v>5</v>
       </c>
       <c r="B675">
-        <v>1013</v>
+        <v>3773</v>
       </c>
       <c r="C675" t="s">
         <v>122</v>
@@ -10255,7 +10255,7 @@
         <v>6</v>
       </c>
       <c r="B676">
-        <v>7427</v>
+        <v>4667</v>
       </c>
       <c r="C676" t="s">
         <v>122</v>
@@ -10325,7 +10325,7 @@
         <v>5</v>
       </c>
       <c r="B681">
-        <v>2034</v>
+        <v>6416</v>
       </c>
       <c r="C681" t="s">
         <v>123</v>
@@ -10339,7 +10339,7 @@
         <v>6</v>
       </c>
       <c r="B682">
-        <v>21388</v>
+        <v>17006</v>
       </c>
       <c r="C682" t="s">
         <v>123</v>
@@ -10409,7 +10409,7 @@
         <v>5</v>
       </c>
       <c r="B687">
-        <v>1666</v>
+        <v>5704</v>
       </c>
       <c r="C687" t="s">
         <v>124</v>
@@ -10423,7 +10423,7 @@
         <v>6</v>
       </c>
       <c r="B688">
-        <v>11424</v>
+        <v>7386</v>
       </c>
       <c r="C688" t="s">
         <v>124</v>
@@ -10493,7 +10493,7 @@
         <v>5</v>
       </c>
       <c r="B693">
-        <v>1311</v>
+        <v>4271</v>
       </c>
       <c r="C693" t="s">
         <v>125</v>
@@ -10507,7 +10507,7 @@
         <v>6</v>
       </c>
       <c r="B694">
-        <v>5129</v>
+        <v>2169</v>
       </c>
       <c r="C694" t="s">
         <v>125</v>
@@ -10577,7 +10577,7 @@
         <v>5</v>
       </c>
       <c r="B699">
-        <v>1553</v>
+        <v>2854</v>
       </c>
       <c r="C699" t="s">
         <v>126</v>
@@ -10591,7 +10591,7 @@
         <v>6</v>
       </c>
       <c r="B700">
-        <v>4011</v>
+        <v>2710</v>
       </c>
       <c r="C700" t="s">
         <v>126</v>
@@ -10661,7 +10661,7 @@
         <v>5</v>
       </c>
       <c r="B705">
-        <v>323</v>
+        <v>1089</v>
       </c>
       <c r="C705" t="s">
         <v>127</v>
@@ -10675,7 +10675,7 @@
         <v>6</v>
       </c>
       <c r="B706">
-        <v>4545</v>
+        <v>3779</v>
       </c>
       <c r="C706" t="s">
         <v>127</v>
@@ -10745,7 +10745,7 @@
         <v>5</v>
       </c>
       <c r="B711">
-        <v>1477</v>
+        <v>4821</v>
       </c>
       <c r="C711" t="s">
         <v>128</v>
@@ -10759,7 +10759,7 @@
         <v>6</v>
       </c>
       <c r="B712">
-        <v>9709</v>
+        <v>6365</v>
       </c>
       <c r="C712" t="s">
         <v>128</v>
@@ -10829,7 +10829,7 @@
         <v>5</v>
       </c>
       <c r="B717">
-        <v>382</v>
+        <v>1483</v>
       </c>
       <c r="C717" t="s">
         <v>129</v>
@@ -10843,7 +10843,7 @@
         <v>6</v>
       </c>
       <c r="B718">
-        <v>3096</v>
+        <v>1995</v>
       </c>
       <c r="C718" t="s">
         <v>129</v>
@@ -10913,7 +10913,7 @@
         <v>5</v>
       </c>
       <c r="B723">
-        <v>387</v>
+        <v>1610</v>
       </c>
       <c r="C723" t="s">
         <v>130</v>
@@ -10927,7 +10927,7 @@
         <v>6</v>
       </c>
       <c r="B724">
-        <v>3074</v>
+        <v>1851</v>
       </c>
       <c r="C724" t="s">
         <v>130</v>
@@ -10997,7 +10997,7 @@
         <v>5</v>
       </c>
       <c r="B729">
-        <v>1666</v>
+        <v>4517</v>
       </c>
       <c r="C729" t="s">
         <v>131</v>
@@ -11011,7 +11011,7 @@
         <v>6</v>
       </c>
       <c r="B730">
-        <v>7477</v>
+        <v>4626</v>
       </c>
       <c r="C730" t="s">
         <v>131</v>
@@ -11081,7 +11081,7 @@
         <v>5</v>
       </c>
       <c r="B735">
-        <v>2728</v>
+        <v>6486</v>
       </c>
       <c r="C735" t="s">
         <v>132</v>
@@ -11095,7 +11095,7 @@
         <v>6</v>
       </c>
       <c r="B736">
-        <v>7876</v>
+        <v>4118</v>
       </c>
       <c r="C736" t="s">
         <v>132</v>
@@ -11165,7 +11165,7 @@
         <v>5</v>
       </c>
       <c r="B741">
-        <v>833</v>
+        <v>2553</v>
       </c>
       <c r="C741" t="s">
         <v>133</v>
@@ -11179,7 +11179,7 @@
         <v>6</v>
       </c>
       <c r="B742">
-        <v>5861</v>
+        <v>4141</v>
       </c>
       <c r="C742" t="s">
         <v>133</v>
@@ -11249,7 +11249,7 @@
         <v>5</v>
       </c>
       <c r="B747">
-        <v>1280</v>
+        <v>4470</v>
       </c>
       <c r="C747" t="s">
         <v>134</v>
@@ -11263,7 +11263,7 @@
         <v>6</v>
       </c>
       <c r="B748">
-        <v>9073</v>
+        <v>5883</v>
       </c>
       <c r="C748" t="s">
         <v>134</v>
@@ -11333,7 +11333,7 @@
         <v>5</v>
       </c>
       <c r="B753">
-        <v>607</v>
+        <v>2099</v>
       </c>
       <c r="C753" t="s">
         <v>135</v>
@@ -11347,7 +11347,7 @@
         <v>6</v>
       </c>
       <c r="B754">
-        <v>3249</v>
+        <v>1757</v>
       </c>
       <c r="C754" t="s">
         <v>135</v>
@@ -11417,7 +11417,7 @@
         <v>5</v>
       </c>
       <c r="B759">
-        <v>1090</v>
+        <v>2727</v>
       </c>
       <c r="C759" t="s">
         <v>136</v>
@@ -11431,7 +11431,7 @@
         <v>6</v>
       </c>
       <c r="B760">
-        <v>4987</v>
+        <v>3350</v>
       </c>
       <c r="C760" t="s">
         <v>136</v>
@@ -11501,7 +11501,7 @@
         <v>5</v>
       </c>
       <c r="B765">
-        <v>79</v>
+        <v>300</v>
       </c>
       <c r="C765" t="s">
         <v>137</v>
@@ -11515,7 +11515,7 @@
         <v>6</v>
       </c>
       <c r="B766">
-        <v>663</v>
+        <v>442</v>
       </c>
       <c r="C766" t="s">
         <v>137</v>
@@ -11585,7 +11585,7 @@
         <v>5</v>
       </c>
       <c r="B771">
-        <v>261</v>
+        <v>1071</v>
       </c>
       <c r="C771" t="s">
         <v>138</v>
@@ -11599,7 +11599,7 @@
         <v>6</v>
       </c>
       <c r="B772">
-        <v>2698</v>
+        <v>1888</v>
       </c>
       <c r="C772" t="s">
         <v>138</v>
@@ -11669,7 +11669,7 @@
         <v>5</v>
       </c>
       <c r="B777">
-        <v>730</v>
+        <v>2005</v>
       </c>
       <c r="C777" t="s">
         <v>139</v>
@@ -11683,7 +11683,7 @@
         <v>6</v>
       </c>
       <c r="B778">
-        <v>4725</v>
+        <v>3450</v>
       </c>
       <c r="C778" t="s">
         <v>139</v>
@@ -11753,7 +11753,7 @@
         <v>5</v>
       </c>
       <c r="B783">
-        <v>692</v>
+        <v>1379</v>
       </c>
       <c r="C783" t="s">
         <v>140</v>
@@ -11767,7 +11767,7 @@
         <v>6</v>
       </c>
       <c r="B784">
-        <v>1866</v>
+        <v>1179</v>
       </c>
       <c r="C784" t="s">
         <v>140</v>

</xml_diff>